<commit_message>
updates to test forward phase of lang rt migration
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-wc_lang-model.xlsx
+++ b/tests/fixtures/example-wc_lang-model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-35720" yWindow="500" windowWidth="26340" windowHeight="18140" tabRatio="993" firstSheet="14" activeTab="23"/>
+    <workbookView xWindow="-28440" yWindow="4640" windowWidth="23640" windowHeight="11220" tabRatio="993" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table of contents" sheetId="23" r:id="rId1"/>
@@ -6520,10 +6520,10 @@
     <t>Url</t>
   </si>
   <si>
-    <t>14e7212a4c7e2421f805ca6f096317d755b4dea0</t>
-  </si>
-  <si>
     <t>https://github.com/KarrLab/wc_lang</t>
+  </si>
+  <si>
+    <t>c14c450d220106e8f0044eef4a8aff687d2c401e</t>
   </si>
 </sst>
 </file>
@@ -6544,31 +6544,26 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6576,19 +6571,16 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
@@ -6693,15 +6685,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6713,6 +6696,15 @@
     <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -11032,11 +11024,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="27" t="s">
         <v>712</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -21684,42 +21676,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView zoomScale="147" zoomScaleNormal="147" zoomScalePageLayoutView="147" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="XFD1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" zoomScalePageLayoutView="147" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="F20" sqref="F20"/>
-      <selection pane="topRight" activeCell="F20" sqref="F20"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="27" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="27" customWidth="1"/>
-    <col min="3" max="3" width="0" style="27" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="0" style="27" hidden="1"/>
+    <col min="1" max="1" width="15.6640625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="24" customWidth="1"/>
+    <col min="3" max="3" width="0" style="24" hidden="1" customWidth="1"/>
+    <col min="4" max="16384" width="0" style="24" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="23" t="s">
         <v>2016</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="25" t="s">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
+        <v>2017</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>2018</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
-        <v>2017</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>2019</v>
       </c>
     </row>
   </sheetData>
@@ -21758,26 +21750,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="28" t="s">
         <v>1802</v>
       </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24" t="s">
+      <c r="H1" s="28"/>
+      <c r="I1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="Q1" s="24" t="s">
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="Q1" s="28" t="s">
         <v>1803</v>
       </c>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24" t="s">
+      <c r="R1" s="28"/>
+      <c r="S1" s="28" t="s">
         <v>1804</v>
       </c>
-      <c r="T1" s="24"/>
+      <c r="T1" s="28"/>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
@@ -22159,10 +22151,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="28" t="s">
         <v>1847</v>
       </c>
-      <c r="H1" s="24"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
@@ -23139,7 +23131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -23666,18 +23658,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="M1" s="22" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="M1" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
     </row>
     <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
@@ -23889,14 +23881,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
update schema repo metadata to commit & branch of new test
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-wc_lang-model.xlsx
+++ b/tests/fixtures/example-wc_lang-model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28440" yWindow="4640" windowWidth="23640" windowHeight="11220" tabRatio="993" activeTab="1"/>
+    <workbookView xWindow="3900" yWindow="680" windowWidth="23640" windowHeight="11220" tabRatio="993" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table of contents" sheetId="23" r:id="rId1"/>
@@ -6514,16 +6514,16 @@
     <t>Intention type</t>
   </si>
   <si>
-    <t>master</t>
-  </si>
-  <si>
     <t>Url</t>
   </si>
   <si>
     <t>https://github.com/KarrLab/wc_lang</t>
   </si>
   <si>
-    <t>c14c450d220106e8f0044eef4a8aff687d2c401e</t>
+    <t>572fc183a267e0530203f38e839b8d996d0a7413</t>
+  </si>
+  <si>
+    <t>migrate_test</t>
   </si>
 </sst>
 </file>
@@ -21679,7 +21679,7 @@
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" zoomScalePageLayoutView="147" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="F20" sqref="F20"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -21695,7 +21695,7 @@
         <v>34</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>2016</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -21703,15 +21703,15 @@
         <v>36</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
+        <v>2016</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>2017</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>2018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>